<commit_message>
Implementada validación de carpetas y configuración de gitignore
</commit_message>
<xml_diff>
--- a/proyecto_cfdi/output_excel/reporte_cfdi.xlsx
+++ b/proyecto_cfdi/output_excel/reporte_cfdi.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,17 +443,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Archivo</t>
+          <t>Fecha</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Fecha</t>
+          <t>Tipo Comprobante</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Tipo Comprobante</t>
+          <t>Metodo de Pago</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -473,173 +473,137 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>tasa_cuota</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>importe</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Moneda</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Emisor RFC</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Emisor Nombre</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Receptor RFC</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Receptor Nombre</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Uso CFDI</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>RegimenFiscalReceptor</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Descripcion</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1a3e0f9a-ec50-4020-bf93-33f613599acb</t>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C:\Users\raulb\OneDrive\Documents Raul\Python\Proyecto extraccion datos CFDI 4.0\proyecto_cfdi\input_cfdi\1a3e0f9a-ec50-4020-bf93-33f613599acb.xml</t>
+          <t>2025-12-31T17:47:06</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-07-26T10:11:30</t>
+          <t>Pago</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>No especificado</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>DZ</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1400608736</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>XXX</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>TME9408297B1</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>TBC DE MEXICO</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>NOCM870307M67</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>MARCO ANTONIO NORIEGA CAMPOS</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>CP01</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>626</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
           <t>Pago</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>DZ</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>1400541269</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>XXX</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>TME9408297B1</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>TBC DE MEXICO</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>NOCM870307M67</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>MARCO ANTONIO NORIEGA CAMPOS</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>CP01</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>A1B2C3D4-E5F6-7890-ABCD-1234567890EF</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>C:\Users\raulb\OneDrive\Documents Raul\Python\Proyecto extraccion datos CFDI 4.0\proyecto_cfdi\input_cfdi\ejemplo_xml_cfdi.xml</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2024-08-15T10:30:25</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Ingreso (Factura)</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>12345</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1160</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>MXN</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>DEMO010101001</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Empresa Demostrativa SA de CV</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>XAXX010101000</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Juan Pérez González</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>G03</t>
         </is>
       </c>
     </row>
@@ -654,7 +618,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -707,7 +671,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1a3e0f9a-ec50-4020-bf93-33f613599acb</t>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -735,74 +699,6 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>A1B2C3D4-E5F6-7890-ABCD-1234567890EF</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>84111506</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>H87</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Servicio de consultoría en tecnología</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>A1B2C3D4-E5F6-7890-ABCD-1234567890EF</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>50211503</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>H87</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Licencia de software</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>500</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -817,7 +713,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -871,21 +767,36 @@
           <t>ImpSaldoInsoluto</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>BaseDR</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>TasaOCuotaDR</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>ImporteDR</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1a3e0f9a-ec50-4020-bf93-33f613599acb</t>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1a3e0f9a-ec50-4020-bf93-33f613599acb</t>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>D065B318-404C-44B8-832E-9362A1EDA58B</t>
+          <t>BB5DD359-5F3B-46F9-844D-07C66AF352FE</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -895,7 +806,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>9095662083</t>
+          <t>9402551638</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -904,29 +815,38 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>2448.57</v>
+        <v>10638.56</v>
       </c>
       <c r="H2" t="n">
-        <v>2448.57</v>
+        <v>10638.56</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>9850.52</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L2" t="n">
+        <v>788.04</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1a3e0f9a-ec50-4020-bf93-33f613599acb</t>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1a3e0f9a-ec50-4020-bf93-33f613599acb</t>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4A3B4874-F687-4434-9DF4-3667E470C942</t>
+          <t>88950E70-73F0-4F95-A80F-5935FFB9545E</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -936,7 +856,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>9095702633</t>
+          <t>9402551802</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -945,29 +865,38 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>770.4299999999999</v>
+        <v>982.64</v>
       </c>
       <c r="H3" t="n">
-        <v>770.4299999999999</v>
+        <v>982.64</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>909.85</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L3" t="n">
+        <v>72.79000000000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1a3e0f9a-ec50-4020-bf93-33f613599acb</t>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1a3e0f9a-ec50-4020-bf93-33f613599acb</t>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>9A474F1B-9A41-477D-800C-4F59500BE0B8</t>
+          <t>0C94D2B4-B7AA-4F6F-901E-8919D6B65444</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -977,7 +906,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>9095732068</t>
+          <t>9402557408</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -986,39 +915,48 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>439.92</v>
+        <v>982.64</v>
       </c>
       <c r="H4" t="n">
-        <v>319.6</v>
+        <v>982.64</v>
       </c>
       <c r="I4" t="n">
-        <v>120.32</v>
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>909.85</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L4" t="n">
+        <v>72.79000000000001</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>A1B2C3D4-E5F6-7890-ABCD-1234567890EF</t>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>A1B2C3D4-E5F6-7890-ABCD-1234567890EF</t>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>A1B2C3D4-E5F6-7890-ABCD-1234567890EF</t>
+          <t>59EB867B-7538-4C60-8654-42F8BF751D73</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>RV</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>12345</t>
+          <t>9402559229</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1027,13 +965,422 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>2320</v>
+        <v>2681.59</v>
       </c>
       <c r="H5" t="n">
-        <v>2320</v>
+        <v>2681.59</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>2482.95</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L5" t="n">
+        <v>198.64</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>B8FE66D6-AB77-416B-99EB-C64DAB8F9D0E</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>RV</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>9402605055</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>MXN</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>788.27</v>
+      </c>
+      <c r="H6" t="n">
+        <v>788.27</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>729.88</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L6" t="n">
+        <v>58.39</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>D752B458-09B9-48FA-9DAB-0B334A311BAD</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>RV</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>9402642523</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>MXN</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>2594.21</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2594.21</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>2402.05</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L7" t="n">
+        <v>192.16</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>8D714DC6-B74B-4A70-AECE-B5E265B69E14</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>RV</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>9402684874</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>MXN</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>1075</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1075</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>995.37</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L8" t="n">
+        <v>79.63</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>D96FD6CB-EF8C-4CC0-BF15-E601B318C9F3</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>RV</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>9402711566</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>MXN</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>718.1</v>
+      </c>
+      <c r="H9" t="n">
+        <v>718.1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>664.91</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L9" t="n">
+        <v>53.19</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>C97FBD67-5B4B-467E-96B9-4D3167295E53</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>RV</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>9402717775</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>MXN</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>439.24</v>
+      </c>
+      <c r="H10" t="n">
+        <v>439.24</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>406.7</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L10" t="n">
+        <v>32.54</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>23982EBD-AF2C-4423-B9C3-21442E97CEA0</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>RV</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>9402717777</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>MXN</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>359.05</v>
+      </c>
+      <c r="H11" t="n">
+        <v>359.05</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>332.45</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L11" t="n">
+        <v>26.6</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>FE512C38-966F-4DF9-B91F-3DC36CD05899</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>RV</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>9402757467</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>MXN</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>5176.59</v>
+      </c>
+      <c r="H12" t="n">
+        <v>5176.59</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>4793.14</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L12" t="n">
+        <v>383.45</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>6555c8ec-ec83-4ba0-bc2b-1b045049a581</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>A944C2D6-F536-4E6F-85E3-26C09489AA72</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>RV</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>9402758534</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>MXN</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>5226.36</v>
+      </c>
+      <c r="H13" t="n">
+        <v>3942.21</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1284.15</v>
+      </c>
+      <c r="J13" t="n">
+        <v>3650.19</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L13" t="n">
+        <v>292.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>